<commit_message>
actualizar análisis: morfología + varianza
</commit_message>
<xml_diff>
--- a/analisis_higado/mejores_modelos.xlsx
+++ b/analisis_higado/mejores_modelos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Dropbox/Transporte_interno/Máster/Ciencia de Datos/TFM/Analisis_final_higado/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Dropbox/Transporte_interno/Máster/Ciencia de Datos/TFM/analisis_higado/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D348D2-33F9-5745-8B59-1855203213F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90A9147-D6C3-E044-B984-96D2E5CB9108}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10640" yWindow="3440" windowWidth="22760" windowHeight="10300" xr2:uid="{E97C1A88-D41F-A846-A94D-29193C2F6B6D}"/>
+    <workbookView xWindow="9120" yWindow="1220" windowWidth="13520" windowHeight="18400" xr2:uid="{E97C1A88-D41F-A846-A94D-29193C2F6B6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
   <si>
     <t>SVM</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>Biclase</t>
-  </si>
-  <si>
-    <t>Multiclase</t>
   </si>
   <si>
     <t>Parámetros</t>
@@ -108,6 +105,28 @@
   </si>
   <si>
     <t>http://onlineconfusionmatrix.com</t>
+  </si>
+  <si>
+    <t>Multiclase estadio</t>
+  </si>
+  <si>
+    <t>Multiclase morfología</t>
+  </si>
+  <si>
+    <t>mrmr 13 genes</t>
+  </si>
+  <si>
+    <t>coste = 1
+gamma = 0.08</t>
+  </si>
+  <si>
+    <t>mrmr 15 genes</t>
+  </si>
+  <si>
+    <t>97,61</t>
+  </si>
+  <si>
+    <t>92,20</t>
   </si>
 </sst>
 </file>
@@ -854,23 +873,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE042987-4404-B845-93EB-ACD32ECBA8D6}">
-  <dimension ref="B1:N7"/>
+  <dimension ref="B1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="9" width="12.1640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13" style="1" customWidth="1"/>
-    <col min="11" max="14" width="12.1640625" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="12.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5" max="8" width="12.1640625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:14" s="2" customFormat="1" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:8" s="2" customFormat="1" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C2" s="28" t="s">
         <v>2</v>
       </c>
@@ -879,62 +899,36 @@
       <c r="F2" s="29"/>
       <c r="G2" s="29"/>
       <c r="H2" s="30"/>
-      <c r="I2" s="28" t="s">
+    </row>
+    <row r="3" spans="2:8" s="2" customFormat="1" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="30"/>
-    </row>
-    <row r="3" spans="2:14" s="2" customFormat="1" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>4</v>
-      </c>
       <c r="E3" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="20" t="s">
-        <v>9</v>
-      </c>
       <c r="G3" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="K3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="M3" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="N3" s="24" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="2:14" s="2" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="2:8" s="2" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="10" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="14">
         <v>99.67</v>
@@ -948,34 +942,16 @@
       <c r="H4" s="15">
         <v>99.13</v>
       </c>
-      <c r="I4" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" s="14">
-        <v>12.91</v>
-      </c>
-      <c r="L4" s="21">
-        <v>78.11</v>
-      </c>
-      <c r="M4" s="13">
-        <v>53.35</v>
-      </c>
-      <c r="N4" s="15">
-        <v>72.48</v>
-      </c>
-    </row>
-    <row r="5" spans="2:14" s="2" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="2:8" s="2" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="3">
         <v>99.67</v>
@@ -989,34 +965,16 @@
       <c r="H5" s="5">
         <v>99.13</v>
       </c>
-      <c r="I5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="3">
-        <v>69.92</v>
-      </c>
-      <c r="L5" s="4">
-        <v>76.319999999999993</v>
-      </c>
-      <c r="M5" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="N5" s="5">
-        <v>61.47</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" s="2" customFormat="1" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:8" s="2" customFormat="1" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="8">
         <v>99.62</v>
@@ -1030,34 +988,217 @@
       <c r="H6" s="9">
         <v>99.13</v>
       </c>
-      <c r="I6" s="7" t="s">
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G7" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:8" s="2" customFormat="1" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="30"/>
+    </row>
+    <row r="10" spans="2:8" s="2" customFormat="1" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" s="2" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="14">
+        <v>95.59</v>
+      </c>
+      <c r="F11" s="21">
+        <v>97.91</v>
+      </c>
+      <c r="G11" s="13">
+        <v>89.57</v>
+      </c>
+      <c r="H11" s="15">
+        <v>95.46</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" s="2" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="3">
+        <v>95.05</v>
+      </c>
+      <c r="F12" s="4">
+        <v>98.21</v>
+      </c>
+      <c r="G12" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="5">
+        <v>96.36</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" s="2" customFormat="1" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="8">
+        <v>94.96</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="7">
+        <v>90.48</v>
+      </c>
+      <c r="H13" s="9">
+        <v>95.46</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:8" s="2" customFormat="1" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="30"/>
+    </row>
+    <row r="16" spans="2:8" s="2" customFormat="1" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" s="24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" s="2" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="14">
+        <v>12.91</v>
+      </c>
+      <c r="F17" s="21">
+        <v>78.11</v>
+      </c>
+      <c r="G17" s="13">
+        <v>53.35</v>
+      </c>
+      <c r="H17" s="15">
+        <v>72.48</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" s="2" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="3">
+        <v>69.92</v>
+      </c>
+      <c r="F18" s="4">
+        <v>76.319999999999993</v>
+      </c>
+      <c r="G18" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="5">
+        <v>61.47</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" s="2" customFormat="1" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="8">
+        <v>64.67</v>
+      </c>
+      <c r="F19" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="K6" s="8">
-        <v>64.67</v>
-      </c>
-      <c r="L6" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="M6" s="7">
+      <c r="G19" s="7">
         <v>65.63</v>
       </c>
-      <c r="N6" s="9">
+      <c r="H19" s="9">
         <v>66.97</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="G7" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
+    <mergeCell ref="C15:H15"/>
     <mergeCell ref="C2:H2"/>
-    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="C9:H9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>